<commit_message>
AG-Zuschuss Pflegeversicherung für PRivat-Versicherte hinzugefügt. Excel mit Quellen für Versicheurngen angelegt.
</commit_message>
<xml_diff>
--- a/src/main/insert personenbezogene Daten/10.1 Mitarbeiter.xlsx
+++ b/src/main/insert personenbezogene Daten/10.1 Mitarbeiter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert personenbezogene Daten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857FDA75-508F-4EA4-B114-4097AC226B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDD9F11-1266-4461-9ADC-185F63A0754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
   <si>
     <t>11 111 111 111</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>31.12.9999</t>
+  </si>
+  <si>
+    <t>Zuschuss private Pflegeversicherung</t>
   </si>
 </sst>
 </file>
@@ -804,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,7 +1147,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1153,34 +1156,42 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>49</v>
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1222,7 +1233,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B28 B41 B37 B45 B46 B32 B40 B38 B43 B44 B34:B36</xm:sqref>
+          <xm:sqref>B28 B32 B40:B41 B44:B47 B34:B38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC540D61-4588-479B-B62B-BA6755FB2963}">
           <x14:formula1>

</xml_diff>